<commit_message>
Add feature: show weather in a few days
</commit_message>
<xml_diff>
--- a/weather.xlsx
+++ b/weather.xlsx
@@ -23321,20 +23321,20 @@
       <c r="A1096" s="2" t="n">
         <v>44472</v>
       </c>
-      <c r="B1096" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1096" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1096" s="50" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1096" s="50" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1096" s="50" t="n">
-        <v>5</v>
+      <c r="B1096" s="51" t="n">
+        <v>22</v>
+      </c>
+      <c r="C1096" s="51" t="n">
+        <v>33</v>
+      </c>
+      <c r="D1096" s="51" t="n">
+        <v>44</v>
+      </c>
+      <c r="E1096" s="51" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1096" s="51" t="n">
+        <v>66</v>
       </c>
       <c r="G1096" s="26" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Refactor again and cut 'open file checker'
</commit_message>
<xml_diff>
--- a/weather.xlsx
+++ b/weather.xlsx
@@ -23366,6 +23366,21 @@
       <c r="A1099" s="2" t="n">
         <v>44475</v>
       </c>
+      <c r="B1099" s="51" t="n">
+        <v>11</v>
+      </c>
+      <c r="C1099" s="51" t="n">
+        <v>22</v>
+      </c>
+      <c r="D1099" s="51" t="n">
+        <v>33</v>
+      </c>
+      <c r="E1099" s="51" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1099" s="51" t="n">
+        <v>55</v>
+      </c>
       <c r="G1099" s="26" t="inlineStr">
         <is>
           <t>06.10.2021</t>

</xml_diff>

<commit_message>
Add check and create config on first start
</commit_message>
<xml_diff>
--- a/weather.xlsx
+++ b/weather.xlsx
@@ -692,7 +692,7 @@
       <selection pane="bottomLeft" activeCell="A2595" sqref="A2595"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" style="2" min="1" max="1"/>
     <col width="14" customWidth="1" style="36" min="2" max="2"/>
@@ -23428,19 +23428,19 @@
         <v>44484</v>
       </c>
       <c r="B1108" s="22" t="n">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="C1108" s="22" t="n">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="D1108" s="22" t="n">
-        <v>3</v>
+        <v>432</v>
       </c>
       <c r="E1108" s="22" t="n">
-        <v>4</v>
+        <v>324</v>
       </c>
       <c r="F1108" s="22" t="n">
-        <v>5</v>
+        <v>322</v>
       </c>
       <c r="M1108" s="31" t="inlineStr">
         <is>
@@ -23452,6 +23452,21 @@
       <c r="A1109" s="2" t="n">
         <v>44485</v>
       </c>
+      <c r="B1109" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="C1109" s="22" t="n">
+        <v>34</v>
+      </c>
+      <c r="D1109" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="E1109" s="22" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1109" s="22" t="n">
+        <v>56</v>
+      </c>
       <c r="M1109" s="31" t="inlineStr">
         <is>
           <t>16.10.2021</t>
@@ -23461,6 +23476,21 @@
     <row r="1110">
       <c r="A1110" s="2" t="n">
         <v>44486</v>
+      </c>
+      <c r="B1110" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1110" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1110" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1110" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1110" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="M1110" s="31" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add function auto create config on start
</commit_message>
<xml_diff>
--- a/weather.xlsx
+++ b/weather.xlsx
@@ -23478,19 +23478,19 @@
         <v>44486</v>
       </c>
       <c r="B1110" s="22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1110" s="22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1110" s="22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E1110" s="22" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1110" s="22" t="n">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="M1110" s="31" t="inlineStr">
         <is>

</xml_diff>